<commit_message>
I Modified some files
</commit_message>
<xml_diff>
--- a/CollegeData.xlsx
+++ b/CollegeData.xlsx
@@ -1,39 +1,233 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\Faculty Projects\Python Project\Students-Pass-System\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E633F5-6455-4E16-BB6B-D4EEDA03F530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Students" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Lecturers" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Students" sheetId="1" r:id="rId1"/>
+    <sheet name="Lecturers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>National Id</t>
+  </si>
+  <si>
+    <t>College Id</t>
+  </si>
+  <si>
+    <t>Departement</t>
+  </si>
+  <si>
+    <t>Vaccination State</t>
+  </si>
+  <si>
+    <t>Current Year</t>
+  </si>
+  <si>
+    <t>Graduation Year</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Mohamed Mamdouh</t>
+  </si>
+  <si>
+    <t>128753</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>vaccinated</t>
+  </si>
+  <si>
+    <t>Second year</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>Main Stream</t>
+  </si>
+  <si>
+    <t>Michael Metry</t>
+  </si>
+  <si>
+    <t>589643</t>
+  </si>
+  <si>
+    <t>21663580</t>
+  </si>
+  <si>
+    <t>Ammar Mohamed</t>
+  </si>
+  <si>
+    <t>589413</t>
+  </si>
+  <si>
+    <t>21663977</t>
+  </si>
+  <si>
+    <t>Mostafa Shoman</t>
+  </si>
+  <si>
+    <t>147320</t>
+  </si>
+  <si>
+    <t>Mohamed Fares</t>
+  </si>
+  <si>
+    <t>259637</t>
+  </si>
+  <si>
+    <t>Mostafa Arabi</t>
+  </si>
+  <si>
+    <t>478561</t>
+  </si>
+  <si>
+    <t>21663548</t>
+  </si>
+  <si>
+    <t>Israa Ibrahim</t>
+  </si>
+  <si>
+    <t>423567</t>
+  </si>
+  <si>
+    <t>Speciality</t>
+  </si>
+  <si>
+    <t>Source University</t>
+  </si>
+  <si>
+    <t>Abdallah Mohamed</t>
+  </si>
+  <si>
+    <t>147652</t>
+  </si>
+  <si>
+    <t>43559630</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>AI - Machine Learning</t>
+  </si>
+  <si>
+    <t>Benha</t>
+  </si>
+  <si>
+    <t>Sabah</t>
+  </si>
+  <si>
+    <t>852456</t>
+  </si>
+  <si>
+    <t>43550089</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Sideq Saqr</t>
+  </si>
+  <si>
+    <t>458329</t>
+  </si>
+  <si>
+    <t>Signals</t>
+  </si>
+  <si>
+    <t>Radwa Sabry</t>
+  </si>
+  <si>
+    <t>478234</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Engineering Mathematics</t>
+  </si>
+  <si>
+    <t>Engy</t>
+  </si>
+  <si>
+    <t>425836</t>
+  </si>
+  <si>
+    <t>43551278</t>
+  </si>
+  <si>
+    <t>Networks</t>
+  </si>
+  <si>
+    <t>Hadeer</t>
+  </si>
+  <si>
+    <t>478532</t>
+  </si>
+  <si>
+    <t>Electromagnetic Fields</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,84 +239,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -410,55 +553,418 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>21664320</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>21669986</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <v>21665749</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1">
+        <v>21663905</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43550196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43552288</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43559610</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I edited some problems
</commit_message>
<xml_diff>
--- a/CollegeData.xlsx
+++ b/CollegeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\Faculty Projects\Python Project\Students-Pass-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E633F5-6455-4E16-BB6B-D4EEDA03F530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA89E5E-6446-49FE-A733-4E49FF33C6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>Electromagnetic Fields</t>
+  </si>
+  <si>
+    <t>Sherief</t>
+  </si>
+  <si>
+    <t>14225365</t>
+  </si>
+  <si>
+    <t>4355632140</t>
+  </si>
+  <si>
+    <t>Field</t>
   </si>
 </sst>
 </file>
@@ -556,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -787,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,6 +976,29 @@
         <v>37</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>